<commit_message>
Added logic/erd-changes for All Stations by year
</commit_message>
<xml_diff>
--- a/resources/column_descriptions.xlsx
+++ b/resources/column_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Data Bootcamp\Homework\Final Project\Home_Gardeners_Analysis\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5210541D-9949-4C42-B0AC-99FF6EE6BDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09C0EA4-AA28-49C1-99B4-BF588828F4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="23264" windowHeight="13695"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="column_descriptions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
   <si>
     <t>Table / View</t>
   </si>
@@ -440,12 +440,57 @@
   </si>
   <si>
     <t>Number of years county had last freeze after average</t>
+  </si>
+  <si>
+    <t>all_stations_yearly_metrics</t>
+  </si>
+  <si>
+    <t>avg_last_freeze_date</t>
+  </si>
+  <si>
+    <t>median_last_freeze_date</t>
+  </si>
+  <si>
+    <t>Coldest day of the year for the full dataset</t>
+  </si>
+  <si>
+    <t>Hottest day of the year for the full dataset</t>
+  </si>
+  <si>
+    <t>Last spring freeze date of all stations in the dataset for the year</t>
+  </si>
+  <si>
+    <t>Last spring freeze date as the "Day of Year"</t>
+  </si>
+  <si>
+    <t>First fall freeze date of all stations in the dataset for the year</t>
+  </si>
+  <si>
+    <t>First fall freeze date as the "Day of Year"</t>
+  </si>
+  <si>
+    <t>Observations recorded April to May</t>
+  </si>
+  <si>
+    <t>Average of all stations' last freeze dates across the year - Day of Year Format</t>
+  </si>
+  <si>
+    <t>Average of all stations' last freeze dates across the year - Calendar Date Format</t>
+  </si>
+  <si>
+    <t>Median of all stations' last freeze dates across the year - Day of Year Format</t>
+  </si>
+  <si>
+    <t>Median of all stations' last freeze dates across the year - Calendar Date Format</t>
+  </si>
+  <si>
+    <t>Number of stations included in the count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -781,7 +826,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -911,6 +956,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -956,12 +1014,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1316,11 +1375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,17 +2497,199 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>